<commit_message>
Cambios de estilos en home
</commit_message>
<xml_diff>
--- a/src/assets/archivos/PPS -4A-2c2017.xlsx
+++ b/src/assets/archivos/PPS -4A-2c2017.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macar\TP_PPS_2C_2017\src\assets\archivos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="18735" windowHeight="8130"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>FINK, Guillermo Federico</t>
   </si>
@@ -106,13 +111,19 @@
   </si>
   <si>
     <t>Sabado  8:30 12:30</t>
+  </si>
+  <si>
+    <t>Sabado  8:30 12:31</t>
+  </si>
+  <si>
+    <t>ALUMNO, Alumno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,11 +190,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -225,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,9 +276,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,6 +328,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,21 +521,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>103295</v>
       </c>
@@ -491,7 +546,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>104286</v>
       </c>
@@ -502,7 +557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>67223</v>
       </c>
@@ -513,7 +568,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>104321</v>
       </c>
@@ -524,7 +579,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>103903</v>
       </c>
@@ -535,7 +590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>105063</v>
       </c>
@@ -546,7 +601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>103924</v>
       </c>
@@ -557,7 +612,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>66503</v>
       </c>
@@ -568,7 +623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>102473</v>
       </c>
@@ -579,7 +634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>104402</v>
       </c>
@@ -590,7 +645,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>104326</v>
       </c>
@@ -601,7 +656,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>103939</v>
       </c>
@@ -612,7 +667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>104300</v>
       </c>
@@ -623,7 +678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>104415</v>
       </c>
@@ -634,7 +689,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>102976</v>
       </c>
@@ -645,7 +700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>103484</v>
       </c>
@@ -656,7 +711,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>104302</v>
       </c>
@@ -667,7 +722,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>910214</v>
       </c>
@@ -678,7 +733,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>103944</v>
       </c>
@@ -689,7 +744,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>102120</v>
       </c>
@@ -700,7 +755,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>103329</v>
       </c>
@@ -711,7 +766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>100921</v>
       </c>
@@ -722,7 +777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>104305</v>
       </c>
@@ -733,7 +788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>104309</v>
       </c>
@@ -744,7 +799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>66384</v>
       </c>
@@ -755,7 +810,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>103333</v>
       </c>
@@ -766,7 +821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>103292</v>
       </c>
@@ -777,7 +832,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>67334</v>
       </c>
@@ -788,7 +843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>67337</v>
       </c>
@@ -797,6 +852,17 @@
       </c>
       <c r="C29" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>121212</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -805,24 +871,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>